<commit_message>
fix format list staff
</commit_message>
<xml_diff>
--- a/src/models/data/expertise.xlsx
+++ b/src/models/data/expertise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85480058-B70A-49CF-AEED-D2CD15D44024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5753F7-25BE-4289-8366-C9D21C5888B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +43,78 @@
   </si>
   <si>
     <t>fb723ca8-832b-448b-8b73-ab8a632c3e84</t>
+  </si>
+  <si>
+    <t>Gan - Mật - Tụy</t>
+  </si>
+  <si>
+    <t>Nha khoa Tổng quát</t>
+  </si>
+  <si>
+    <t>Cơ Xương Khớp</t>
+  </si>
+  <si>
+    <t>Ung bướu-Xạ trị</t>
+  </si>
+  <si>
+    <t>Y học tái tạo</t>
+  </si>
+  <si>
+    <t>Hồi sức - Cấp cứu</t>
+  </si>
+  <si>
+    <t>Chẩn đoán hình ảnh</t>
+  </si>
+  <si>
+    <t>Tiêu hóa</t>
+  </si>
+  <si>
+    <t>Da liễu</t>
+  </si>
+  <si>
+    <t>Cơ xương khớp</t>
+  </si>
+  <si>
+    <t>Tim mạch</t>
+  </si>
+  <si>
+    <t>Phẫu Thuật chỉnh hình</t>
+  </si>
+  <si>
+    <t>1a7b0d10-4499-4c4b-bd04-529ea20a0846</t>
+  </si>
+  <si>
+    <t>3a076763-c856-4143-a214-67842ea7703c</t>
+  </si>
+  <si>
+    <t>526453d1-ab32-4bca-bea1-ce859b98c56a</t>
+  </si>
+  <si>
+    <t>f2a52eca-9703-435b-8e8e-d6f2f841430a</t>
+  </si>
+  <si>
+    <t>b68c9a33-6c0c-49d4-87e7-a67f85c7856e</t>
+  </si>
+  <si>
+    <t>bb5bba1d-1899-4fe7-a2dd-32fc60cebe38</t>
+  </si>
+  <si>
+    <t>e41b1a6f-2d65-49d4-8af9-59159a0c374c</t>
+  </si>
+  <si>
+    <t>b9238e62-1a0d-4c2a-b98f-a3420ff1f463</t>
+  </si>
+  <si>
+    <t>eba9a698-8741-4712-b71c-8cbbd6ed5734</t>
+  </si>
+  <si>
+    <t>a194a592-7566-4077-a593-e292b51b9151</t>
+  </si>
+  <si>
+    <t>fdd9d6f5-68d2-4923-9895-808d976f5dd1</t>
+  </si>
+  <si>
+    <t>0c1d30e2-f9e4-4588-b85a-3211097b2f1c</t>
   </si>
 </sst>
 </file>
@@ -360,16 +432,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:B3"/>
+      <selection activeCell="A4" sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -396,7 +468,118 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://vinmec.com/vi/chuyen-khoa/gan-mat-tuy-416/" xr:uid="{7CCDAF9C-8704-4569-AD79-01BC7C9F0C47}"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://vinmec.com/vi/chuyen-khoa/nha-khoa-tong-quat-233/" xr:uid="{0F277F14-2446-43D4-9227-ABB33046A78E}"/>
+    <hyperlink ref="B6" r:id="rId3" display="https://vinmec.com/vi/chuyen-khoa/ngoai-co-xuong-khop-230/" xr:uid="{16A191CB-EB78-4B57-927E-7CB60C3BEA0F}"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://vinmec.com/vi/chuyen-khoa/ung-buou-265/" xr:uid="{4633059F-EEF7-4875-ADBB-009E5671B020}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://vinmec.com/vi/chuyen-khoa/tu-ky-bai-nao-415/" xr:uid="{14291009-D719-488A-B9F9-8C5EDFC9C73A}"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://vinmec.com/vi/chuyen-khoa/hoi-suc-cap-cuu-223/" xr:uid="{33BCDE3E-D1B0-4F84-BA62-665A5EE9C676}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://vinmec.com/vi/chuyen-khoa/chan-doan-hinh-anh-288/" xr:uid="{C843EC2C-0745-4889-9E08-2CA77A87E12B}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://vinmec.com/vi/chuyen-khoa/tieu-hoa-gan-mat-249/" xr:uid="{03E42FCA-FFB7-448A-BB06-FC3AFF6E9737}"/>
+    <hyperlink ref="B12" r:id="rId9" display="https://vinmec.com/vi/chuyen-khoa/da-lieu-236/" xr:uid="{559732E9-FF09-495F-AB31-60A174AFE674}"/>
+    <hyperlink ref="B13" r:id="rId10" display="https://vinmec.com/vi/chuyen-khoa/co-xuong-khop-227/" xr:uid="{8299ABE5-0261-4F26-95A1-50A844D1283C}"/>
+    <hyperlink ref="B14" r:id="rId11" display="https://vinmec.com/vi/chuyen-khoa/tim-mach-252/" xr:uid="{8B772F3C-B5C1-4094-9651-C479FAD64721}"/>
+    <hyperlink ref="B15" r:id="rId12" display="https://vinmec.com/vi/chuyen-khoa/chan-thuong-chinh-hinh-cot-song-260/" xr:uid="{9869B839-3A1A-480E-9FCD-BDD35210CD92}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add price in expertise
</commit_message>
<xml_diff>
--- a/src/models/data/expertise.xlsx
+++ b/src/models/data/expertise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindonut\Documents\GitHub\Final\MEDRE_BE\src\models\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA877F17-C07F-4766-AE6B-054E03739A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B794AF8B-7E20-453E-B491-62CAC07C4D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1596" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>5e51b358-2ac1-4f46-94c1-d0bc9e1dec07</t>
+  </si>
+  <si>
+    <t>price_offline</t>
+  </si>
+  <si>
+    <t>price_online</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,116 +444,200 @@
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>100000</v>
+      </c>
+      <c r="D3">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>100000</v>
+      </c>
+      <c r="D4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>100000</v>
+      </c>
+      <c r="D5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>100000</v>
+      </c>
+      <c r="D6">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>100000</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>100000</v>
+      </c>
+      <c r="D8">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>100000</v>
+      </c>
+      <c r="D9">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>100000</v>
+      </c>
+      <c r="D10">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>100000</v>
+      </c>
+      <c r="D11">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>100000</v>
+      </c>
+      <c r="D12">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>100000</v>
+      </c>
+      <c r="D13">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
+      </c>
+      <c r="C14">
+        <v>100000</v>
+      </c>
+      <c r="D14">
+        <v>180000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>